<commit_message>
Secon table meta info and update Bewhoner
</commit_message>
<xml_diff>
--- a/data/Bewohner.xlsx
+++ b/data/Bewohner.xlsx
@@ -5,12 +5,12 @@
   <workbookPr defaultThemeVersion="166925"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayumi\Documents\Visual Studio 2017\app\data\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\ayumi\Documents\GitHub\eayumi.github.io\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{84EF83A4-B739-449A-BCBA-39E7D4963064}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{D34A8D06-C234-4DC9-A522-9ADA8029F70B}" xr6:coauthVersionLast="45" xr6:coauthVersionMax="45" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-98" yWindow="-98" windowWidth="19396" windowHeight="10546" xr2:uid="{09F0A162-F573-F644-9F73-AFDCEDDCC34A}"/>
+    <workbookView xWindow="322" yWindow="353" windowWidth="18878" windowHeight="9997" xr2:uid="{09F0A162-F573-F644-9F73-AFDCEDDCC34A}"/>
   </bookViews>
   <sheets>
     <sheet name="Übersicht" sheetId="1" r:id="rId1"/>
@@ -32,7 +32,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="685" uniqueCount="269">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="751" uniqueCount="293">
   <si>
     <t>Soziologe, research ass ETH Wohnforum</t>
   </si>
@@ -832,13 +832,85 @@
     <t>Begabtenforderung</t>
   </si>
   <si>
-    <t>Ubersetzerin, Admin ETH</t>
-  </si>
-  <si>
     <t>Arztin, Rentnerin</t>
   </si>
   <si>
     <t>Week_Year</t>
+  </si>
+  <si>
+    <t>52-20</t>
+  </si>
+  <si>
+    <t>Geschaftsfuhrer</t>
+  </si>
+  <si>
+    <t>Person 35</t>
+  </si>
+  <si>
+    <t>Person 40</t>
+  </si>
+  <si>
+    <t>Hochbauzeichnerin</t>
+  </si>
+  <si>
+    <t>Enkelkinderbetreung</t>
+  </si>
+  <si>
+    <t>Person 42.2</t>
+  </si>
+  <si>
+    <t>Informatiker, Häuser Umbau</t>
+  </si>
+  <si>
+    <t>Person 42.1</t>
+  </si>
+  <si>
+    <t>Person 43.1</t>
+  </si>
+  <si>
+    <t>Verwaltungsangestellte</t>
+  </si>
+  <si>
+    <t>Bad, Küche</t>
+  </si>
+  <si>
+    <t>Person 43.2</t>
+  </si>
+  <si>
+    <t>Beamter</t>
+  </si>
+  <si>
+    <t>Person 45.2</t>
+  </si>
+  <si>
+    <t>Person 49.1</t>
+  </si>
+  <si>
+    <t>Person 49.2</t>
+  </si>
+  <si>
+    <t>Person 48.1</t>
+  </si>
+  <si>
+    <t>ZHDK</t>
+  </si>
+  <si>
+    <t>Pensioniert</t>
+  </si>
+  <si>
+    <t>Person 39.1</t>
+  </si>
+  <si>
+    <t>Naturwissenschaftlerin ETH pensioniert</t>
+  </si>
+  <si>
+    <t>Person 39.2</t>
+  </si>
+  <si>
+    <t>Architekt, Ergotherapeut, pensioniert</t>
+  </si>
+  <si>
+    <t>Vize-Präsident Forschung</t>
   </si>
 </sst>
 </file>
@@ -901,7 +973,7 @@
       <scheme val="minor"/>
     </font>
   </fonts>
-  <fills count="8">
+  <fills count="9">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -944,8 +1016,14 @@
         <bgColor indexed="64"/>
       </patternFill>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="10">
+  <borders count="9">
     <border>
       <left/>
       <right/>
@@ -1043,24 +1121,11 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right style="thin">
-        <color indexed="64"/>
-      </right>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom style="thin">
-        <color indexed="64"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="1">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
   </cellStyleXfs>
-  <cellXfs count="69">
+  <cellXfs count="71">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
@@ -1085,10 +1150,8 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="4" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="3" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="2" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="2" borderId="1" xfId="0" applyFill="1" applyBorder="1"/>
@@ -1120,8 +1183,6 @@
     <xf numFmtId="0" fontId="4" fillId="0" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="0" fillId="3" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="2" fillId="0" borderId="8" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="0" borderId="4" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="4" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="3" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
@@ -1130,8 +1191,14 @@
     <xf numFmtId="49" fontId="2" fillId="7" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="2" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="49" fontId="2" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="49" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="4" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="4" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="2" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="2" fillId="4" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="49" fontId="0" fillId="8" borderId="0" xfId="0" applyNumberFormat="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="2" fillId="7" borderId="0" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="3" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
   </cellXfs>
   <cellStyles count="1">
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
@@ -1449,16 +1516,16 @@
   <sheetPr>
     <pageSetUpPr fitToPage="1"/>
   </sheetPr>
-  <dimension ref="A1:W71"/>
+  <dimension ref="A1:W72"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="58" zoomScaleNormal="113" workbookViewId="0">
+    <sheetView tabSelected="1" topLeftCell="A50" zoomScale="56" zoomScaleNormal="113" workbookViewId="0">
       <pane xSplit="1" topLeftCell="B1" activePane="topRight" state="frozen"/>
-      <selection pane="topRight"/>
+      <selection pane="topRight" activeCell="J80" sqref="J80"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultColWidth="11" defaultRowHeight="15.75"/>
   <cols>
-    <col min="1" max="1" width="12.1875" style="68" customWidth="1"/>
+    <col min="1" max="1" width="12.1875" style="63" customWidth="1"/>
     <col min="2" max="2" width="11.8125" customWidth="1"/>
     <col min="3" max="3" width="10" customWidth="1"/>
     <col min="4" max="4" width="37.3125" customWidth="1"/>
@@ -1478,8 +1545,8 @@
   </cols>
   <sheetData>
     <row r="1" spans="1:23">
-      <c r="A1" s="63" t="s">
-        <v>268</v>
+      <c r="A1" s="59" t="s">
+        <v>267</v>
       </c>
       <c r="B1" s="2" t="s">
         <v>215</v>
@@ -1545,7 +1612,7 @@
       <c r="W1" s="2"/>
     </row>
     <row r="2" spans="1:23">
-      <c r="A2" s="64" t="s">
+      <c r="A2" s="60" t="s">
         <v>149</v>
       </c>
       <c r="B2" s="2" t="s">
@@ -1574,7 +1641,7 @@
       <c r="W2" s="6"/>
     </row>
     <row r="3" spans="1:23">
-      <c r="A3" s="64" t="s">
+      <c r="A3" s="60" t="s">
         <v>150</v>
       </c>
       <c r="B3" s="2" t="s">
@@ -1603,7 +1670,7 @@
       <c r="W3" s="6"/>
     </row>
     <row r="4" spans="1:23">
-      <c r="A4" s="64" t="s">
+      <c r="A4" s="60" t="s">
         <v>151</v>
       </c>
       <c r="B4" s="2" t="s">
@@ -1632,7 +1699,7 @@
       <c r="W4" s="8"/>
     </row>
     <row r="5" spans="1:23">
-      <c r="A5" s="65" t="s">
+      <c r="A5" s="61" t="s">
         <v>152</v>
       </c>
       <c r="B5" s="3" t="s">
@@ -1661,7 +1728,7 @@
       <c r="W5" s="6"/>
     </row>
     <row r="6" spans="1:23">
-      <c r="A6" s="66" t="s">
+      <c r="A6" s="62" t="s">
         <v>153</v>
       </c>
       <c r="B6" s="10" t="s">
@@ -1708,7 +1775,7 @@
       <c r="W6" s="6"/>
     </row>
     <row r="7" spans="1:23">
-      <c r="A7" s="66" t="s">
+      <c r="A7" s="62" t="s">
         <v>154</v>
       </c>
       <c r="B7" s="10" t="s">
@@ -1755,7 +1822,7 @@
       <c r="W7" s="6"/>
     </row>
     <row r="8" spans="1:23">
-      <c r="A8" s="66" t="s">
+      <c r="A8" s="62" t="s">
         <v>155</v>
       </c>
       <c r="B8" s="2" t="s">
@@ -1784,7 +1851,7 @@
       <c r="W8" s="8"/>
     </row>
     <row r="9" spans="1:23">
-      <c r="A9" s="66" t="s">
+      <c r="A9" s="62" t="s">
         <v>156</v>
       </c>
       <c r="B9" s="12" t="s">
@@ -1851,7 +1918,7 @@
       <c r="W9" s="14"/>
     </row>
     <row r="10" spans="1:23">
-      <c r="A10" s="66" t="s">
+      <c r="A10" s="62" t="s">
         <v>157</v>
       </c>
       <c r="B10" s="11" t="s">
@@ -1918,7 +1985,7 @@
       <c r="W10" s="6"/>
     </row>
     <row r="11" spans="1:23">
-      <c r="A11" s="66" t="s">
+      <c r="A11" s="62" t="s">
         <v>158</v>
       </c>
       <c r="B11" s="2" t="s">
@@ -1947,7 +2014,7 @@
       <c r="W11" s="8"/>
     </row>
     <row r="12" spans="1:23">
-      <c r="A12" s="66" t="s">
+      <c r="A12" s="62" t="s">
         <v>159</v>
       </c>
       <c r="B12" s="12" t="s">
@@ -1971,7 +2038,7 @@
       <c r="H12" s="12" t="s">
         <v>137</v>
       </c>
-      <c r="I12" s="36">
+      <c r="I12" s="34">
         <v>5</v>
       </c>
       <c r="J12" s="12" t="s">
@@ -2014,7 +2081,7 @@
       <c r="W12" s="16"/>
     </row>
     <row r="13" spans="1:23">
-      <c r="A13" s="66" t="s">
+      <c r="A13" s="62" t="s">
         <v>160</v>
       </c>
       <c r="B13" s="12" t="s">
@@ -2081,7 +2148,7 @@
       <c r="W13" s="16"/>
     </row>
     <row r="14" spans="1:23">
-      <c r="A14" s="66" t="s">
+      <c r="A14" s="62" t="s">
         <v>161</v>
       </c>
       <c r="B14" s="12" t="s">
@@ -2148,7 +2215,7 @@
       <c r="W14" s="16"/>
     </row>
     <row r="15" spans="1:23">
-      <c r="A15" s="66" t="s">
+      <c r="A15" s="62" t="s">
         <v>162</v>
       </c>
       <c r="B15" s="12" t="s">
@@ -2195,7 +2262,7 @@
       <c r="W15" s="16"/>
     </row>
     <row r="16" spans="1:23">
-      <c r="A16" s="66" t="s">
+      <c r="A16" s="62" t="s">
         <v>163</v>
       </c>
       <c r="B16" s="12" t="s">
@@ -2258,13 +2325,13 @@
       <c r="W16" s="8"/>
     </row>
     <row r="17" spans="1:23">
-      <c r="A17" s="66" t="s">
+      <c r="A17" s="62" t="s">
         <v>164</v>
       </c>
       <c r="B17" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C17" s="34"/>
+      <c r="C17" s="32"/>
       <c r="D17" s="3"/>
       <c r="E17" s="3"/>
       <c r="F17" s="3"/>
@@ -2276,7 +2343,7 @@
       <c r="L17" s="3"/>
       <c r="M17" s="3"/>
       <c r="N17" s="3"/>
-      <c r="O17" s="37"/>
+      <c r="O17" s="35"/>
       <c r="P17" s="3"/>
       <c r="Q17" s="3"/>
       <c r="R17" s="3"/>
@@ -2287,13 +2354,13 @@
       <c r="W17" s="8"/>
     </row>
     <row r="18" spans="1:23">
-      <c r="A18" s="66" t="s">
+      <c r="A18" s="62" t="s">
         <v>165</v>
       </c>
       <c r="B18" s="2" t="s">
         <v>238</v>
       </c>
-      <c r="C18" s="34"/>
+      <c r="C18" s="32"/>
       <c r="D18" s="3"/>
       <c r="E18" s="3"/>
       <c r="F18" s="3"/>
@@ -2316,7 +2383,7 @@
       <c r="W18" s="16"/>
     </row>
     <row r="19" spans="1:23">
-      <c r="A19" s="66" t="s">
+      <c r="A19" s="62" t="s">
         <v>166</v>
       </c>
       <c r="B19" s="2" t="s">
@@ -2324,13 +2391,13 @@
       </c>
       <c r="C19" s="3"/>
       <c r="D19" s="3"/>
-      <c r="E19" s="34"/>
-      <c r="F19" s="34"/>
-      <c r="G19" s="34"/>
-      <c r="H19" s="34"/>
-      <c r="I19" s="34"/>
-      <c r="J19" s="34"/>
-      <c r="K19" s="34"/>
+      <c r="E19" s="32"/>
+      <c r="F19" s="32"/>
+      <c r="G19" s="32"/>
+      <c r="H19" s="32"/>
+      <c r="I19" s="32"/>
+      <c r="J19" s="32"/>
+      <c r="K19" s="32"/>
       <c r="L19" s="3"/>
       <c r="M19" s="3"/>
       <c r="N19" s="3"/>
@@ -2345,7 +2412,7 @@
       <c r="W19" s="16"/>
     </row>
     <row r="20" spans="1:23">
-      <c r="A20" s="66" t="s">
+      <c r="A20" s="62" t="s">
         <v>167</v>
       </c>
       <c r="B20" s="2" t="s">
@@ -2374,7 +2441,7 @@
       <c r="W20" s="16"/>
     </row>
     <row r="21" spans="1:23">
-      <c r="A21" s="66" t="s">
+      <c r="A21" s="62" t="s">
         <v>168</v>
       </c>
       <c r="B21" s="2" t="s">
@@ -2403,7 +2470,7 @@
       <c r="W21" s="16"/>
     </row>
     <row r="22" spans="1:23">
-      <c r="A22" s="66" t="s">
+      <c r="A22" s="62" t="s">
         <v>169</v>
       </c>
       <c r="B22" s="11" t="s">
@@ -2450,7 +2517,7 @@
       <c r="W22" s="16"/>
     </row>
     <row r="23" spans="1:23">
-      <c r="A23" s="66" t="s">
+      <c r="A23" s="62" t="s">
         <v>170</v>
       </c>
       <c r="B23" s="2" t="s">
@@ -2458,28 +2525,28 @@
       </c>
       <c r="C23" s="3"/>
       <c r="D23" s="3"/>
-      <c r="E23" s="33"/>
-      <c r="F23" s="61"/>
-      <c r="G23" s="61"/>
-      <c r="H23" s="61"/>
-      <c r="I23" s="34"/>
-      <c r="J23" s="35"/>
-      <c r="K23" s="35"/>
+      <c r="E23" s="31"/>
+      <c r="F23" s="57"/>
+      <c r="G23" s="57"/>
+      <c r="H23" s="57"/>
+      <c r="I23" s="32"/>
+      <c r="J23" s="33"/>
+      <c r="K23" s="33"/>
       <c r="L23" s="3"/>
       <c r="M23" s="3"/>
       <c r="N23" s="3"/>
       <c r="O23" s="3"/>
-      <c r="P23" s="33"/>
-      <c r="Q23" s="61"/>
-      <c r="R23" s="61"/>
-      <c r="S23" s="34"/>
-      <c r="T23" s="35"/>
-      <c r="U23" s="35"/>
+      <c r="P23" s="31"/>
+      <c r="Q23" s="57"/>
+      <c r="R23" s="57"/>
+      <c r="S23" s="32"/>
+      <c r="T23" s="33"/>
+      <c r="U23" s="33"/>
       <c r="V23" s="16"/>
       <c r="W23" s="16"/>
     </row>
     <row r="24" spans="1:23">
-      <c r="A24" s="66" t="s">
+      <c r="A24" s="62" t="s">
         <v>171</v>
       </c>
       <c r="B24" s="2" t="s">
@@ -2487,13 +2554,13 @@
       </c>
       <c r="C24" s="3"/>
       <c r="D24" s="3"/>
-      <c r="E24" s="33"/>
-      <c r="F24" s="61"/>
-      <c r="G24" s="61"/>
-      <c r="H24" s="61"/>
-      <c r="I24" s="34"/>
-      <c r="J24" s="34"/>
-      <c r="K24" s="34"/>
+      <c r="E24" s="31"/>
+      <c r="F24" s="57"/>
+      <c r="G24" s="57"/>
+      <c r="H24" s="57"/>
+      <c r="I24" s="32"/>
+      <c r="J24" s="32"/>
+      <c r="K24" s="32"/>
       <c r="L24" s="3"/>
       <c r="M24" s="3"/>
       <c r="N24" s="3"/>
@@ -2508,7 +2575,7 @@
       <c r="W24" s="16"/>
     </row>
     <row r="25" spans="1:23">
-      <c r="A25" s="66" t="s">
+      <c r="A25" s="62" t="s">
         <v>172</v>
       </c>
       <c r="B25" s="2" t="s">
@@ -2516,28 +2583,28 @@
       </c>
       <c r="C25" s="3"/>
       <c r="D25" s="3"/>
-      <c r="E25" s="33"/>
-      <c r="F25" s="61"/>
-      <c r="G25" s="61"/>
-      <c r="H25" s="61"/>
-      <c r="I25" s="34"/>
-      <c r="J25" s="34"/>
-      <c r="K25" s="34"/>
+      <c r="E25" s="31"/>
+      <c r="F25" s="57"/>
+      <c r="G25" s="57"/>
+      <c r="H25" s="57"/>
+      <c r="I25" s="32"/>
+      <c r="J25" s="32"/>
+      <c r="K25" s="32"/>
       <c r="L25" s="3"/>
       <c r="M25" s="3"/>
       <c r="N25" s="3"/>
       <c r="O25" s="3"/>
-      <c r="P25" s="34"/>
-      <c r="Q25" s="34"/>
-      <c r="R25" s="34"/>
-      <c r="S25" s="34"/>
-      <c r="T25" s="34"/>
-      <c r="U25" s="34"/>
+      <c r="P25" s="32"/>
+      <c r="Q25" s="32"/>
+      <c r="R25" s="32"/>
+      <c r="S25" s="32"/>
+      <c r="T25" s="32"/>
+      <c r="U25" s="32"/>
       <c r="V25" s="16"/>
       <c r="W25" s="16"/>
     </row>
     <row r="26" spans="1:23">
-      <c r="A26" s="66" t="s">
+      <c r="A26" s="62" t="s">
         <v>173</v>
       </c>
       <c r="B26" s="17" t="s">
@@ -2584,7 +2651,7 @@
       <c r="W26" s="16"/>
     </row>
     <row r="27" spans="1:23">
-      <c r="A27" s="66" t="s">
+      <c r="A27" s="62" t="s">
         <v>174</v>
       </c>
       <c r="B27" s="11" t="s">
@@ -2631,7 +2698,7 @@
       <c r="W27" s="16"/>
     </row>
     <row r="28" spans="1:23">
-      <c r="A28" s="66" t="s">
+      <c r="A28" s="62" t="s">
         <v>175</v>
       </c>
       <c r="B28" s="11" t="s">
@@ -2665,9 +2732,9 @@
         <v>254</v>
       </c>
       <c r="L28" s="3"/>
-      <c r="M28" s="33"/>
-      <c r="N28" s="33"/>
-      <c r="O28" s="33"/>
+      <c r="M28" s="31"/>
+      <c r="N28" s="31"/>
+      <c r="O28" s="31"/>
       <c r="P28" s="3"/>
       <c r="Q28" s="3"/>
       <c r="R28" s="3"/>
@@ -2678,7 +2745,7 @@
       <c r="W28" s="16"/>
     </row>
     <row r="29" spans="1:23">
-      <c r="A29" s="66" t="s">
+      <c r="A29" s="62" t="s">
         <v>177</v>
       </c>
       <c r="B29" s="12" t="s">
@@ -2745,7 +2812,7 @@
       <c r="W29" s="16"/>
     </row>
     <row r="30" spans="1:23">
-      <c r="A30" s="66" t="s">
+      <c r="A30" s="62" t="s">
         <v>176</v>
       </c>
       <c r="B30" s="11" t="s">
@@ -2782,17 +2849,17 @@
       <c r="M30" s="3"/>
       <c r="N30" s="3"/>
       <c r="O30" s="3"/>
-      <c r="P30" s="34"/>
-      <c r="Q30" s="34"/>
-      <c r="R30" s="34"/>
+      <c r="P30" s="32"/>
+      <c r="Q30" s="32"/>
+      <c r="R30" s="32"/>
       <c r="S30" s="21"/>
-      <c r="T30" s="35"/>
-      <c r="U30" s="35"/>
+      <c r="T30" s="33"/>
+      <c r="U30" s="33"/>
       <c r="V30" s="16"/>
       <c r="W30" s="14"/>
     </row>
     <row r="31" spans="1:23">
-      <c r="A31" s="66" t="s">
+      <c r="A31" s="62" t="s">
         <v>178</v>
       </c>
       <c r="B31" s="12" t="s">
@@ -2859,7 +2926,7 @@
       <c r="W31" s="14"/>
     </row>
     <row r="32" spans="1:23">
-      <c r="A32" s="66" t="s">
+      <c r="A32" s="62" t="s">
         <v>179</v>
       </c>
       <c r="B32" s="2" t="s">
@@ -2888,7 +2955,7 @@
       <c r="W32" s="20"/>
     </row>
     <row r="33" spans="1:23">
-      <c r="A33" s="66" t="s">
+      <c r="A33" s="62" t="s">
         <v>180</v>
       </c>
       <c r="B33" s="2" t="s">
@@ -2917,7 +2984,7 @@
       <c r="W33" s="20"/>
     </row>
     <row r="34" spans="1:23">
-      <c r="A34" s="66" t="s">
+      <c r="A34" s="62" t="s">
         <v>181</v>
       </c>
       <c r="B34" s="2" t="s">
@@ -2946,7 +3013,7 @@
       <c r="W34" s="20"/>
     </row>
     <row r="35" spans="1:23">
-      <c r="A35" s="66" t="s">
+      <c r="A35" s="62" t="s">
         <v>182</v>
       </c>
       <c r="B35" s="2" t="s">
@@ -2975,7 +3042,7 @@
       <c r="W35" s="20"/>
     </row>
     <row r="36" spans="1:23">
-      <c r="A36" s="66" t="s">
+      <c r="A36" s="62" t="s">
         <v>183</v>
       </c>
       <c r="B36" s="2" t="s">
@@ -3004,7 +3071,7 @@
       <c r="W36" s="20"/>
     </row>
     <row r="37" spans="1:23">
-      <c r="A37" s="66" t="s">
+      <c r="A37" s="62" t="s">
         <v>184</v>
       </c>
       <c r="B37" s="2" t="s">
@@ -3033,7 +3100,7 @@
       <c r="W37" s="20"/>
     </row>
     <row r="38" spans="1:23">
-      <c r="A38" s="66" t="s">
+      <c r="A38" s="62" t="s">
         <v>147</v>
       </c>
       <c r="B38" s="2" t="s">
@@ -3062,7 +3129,7 @@
       <c r="W38" s="20"/>
     </row>
     <row r="39" spans="1:23">
-      <c r="A39" s="66" t="s">
+      <c r="A39" s="62" t="s">
         <v>185</v>
       </c>
       <c r="B39" s="11" t="s">
@@ -3071,7 +3138,7 @@
       <c r="C39" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D39" s="30" t="s">
+      <c r="D39" s="28" t="s">
         <v>1</v>
       </c>
       <c r="E39" s="10" t="s">
@@ -3104,16 +3171,16 @@
       <c r="N39" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O39" s="30" t="s">
+      <c r="O39" s="28" t="s">
         <v>83</v>
       </c>
-      <c r="P39" s="46" t="s">
+      <c r="P39" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="Q39" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="R39" s="46" t="s">
+      <c r="Q39" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="R39" s="44" t="s">
         <v>139</v>
       </c>
       <c r="S39" s="10">
@@ -3129,7 +3196,7 @@
       <c r="W39" s="20"/>
     </row>
     <row r="40" spans="1:23">
-      <c r="A40" s="66" t="s">
+      <c r="A40" s="62" t="s">
         <v>186</v>
       </c>
       <c r="B40" s="11" t="s">
@@ -3138,7 +3205,7 @@
       <c r="C40" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D40" s="30" t="s">
+      <c r="D40" s="28" t="s">
         <v>118</v>
       </c>
       <c r="E40" s="10" t="s">
@@ -3171,16 +3238,16 @@
       <c r="N40" s="11" t="s">
         <v>5</v>
       </c>
-      <c r="O40" s="43" t="s">
+      <c r="O40" s="41" t="s">
         <v>84</v>
       </c>
-      <c r="P40" s="46" t="s">
+      <c r="P40" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="Q40" s="46" t="s">
+      <c r="Q40" s="44" t="s">
         <v>135</v>
       </c>
-      <c r="R40" s="46" t="s">
+      <c r="R40" s="44" t="s">
         <v>143</v>
       </c>
       <c r="S40" s="10">
@@ -3196,7 +3263,7 @@
       <c r="W40" s="20"/>
     </row>
     <row r="41" spans="1:23">
-      <c r="A41" s="66" t="s">
+      <c r="A41" s="62" t="s">
         <v>187</v>
       </c>
       <c r="B41" s="2" t="s">
@@ -3215,9 +3282,9 @@
       <c r="M41" s="2"/>
       <c r="N41" s="2"/>
       <c r="O41" s="2"/>
-      <c r="P41" s="47"/>
-      <c r="Q41" s="47"/>
-      <c r="R41" s="47"/>
+      <c r="P41" s="45"/>
+      <c r="Q41" s="45"/>
+      <c r="R41" s="45"/>
       <c r="S41" s="2"/>
       <c r="T41" s="2"/>
       <c r="U41" s="2"/>
@@ -3225,7 +3292,7 @@
       <c r="W41" s="20"/>
     </row>
     <row r="42" spans="1:23">
-      <c r="A42" s="66" t="s">
+      <c r="A42" s="62" t="s">
         <v>188</v>
       </c>
       <c r="B42" s="11" t="s">
@@ -3234,7 +3301,7 @@
       <c r="C42" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D42" s="53" t="s">
+      <c r="D42" s="51" t="s">
         <v>86</v>
       </c>
       <c r="E42" s="11" t="s">
@@ -3270,16 +3337,16 @@
       <c r="O42" s="19" t="s">
         <v>87</v>
       </c>
-      <c r="P42" s="44" t="s">
+      <c r="P42" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q42" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R42" s="44" t="s">
+      <c r="Q42" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="R42" s="42" t="s">
         <v>146</v>
       </c>
-      <c r="S42" s="25">
+      <c r="S42" s="24">
         <v>9</v>
       </c>
       <c r="T42" s="19" t="s">
@@ -3289,10 +3356,10 @@
         <v>251</v>
       </c>
       <c r="V42" s="20"/>
-      <c r="W42" s="32"/>
+      <c r="W42" s="30"/>
     </row>
     <row r="43" spans="1:23">
-      <c r="A43" s="66" t="s">
+      <c r="A43" s="62" t="s">
         <v>189</v>
       </c>
       <c r="B43" s="2" t="s">
@@ -3308,19 +3375,19 @@
       <c r="J43" s="21"/>
       <c r="K43" s="21"/>
       <c r="L43" s="8"/>
-      <c r="M43" s="31"/>
-      <c r="N43" s="62"/>
-      <c r="P43" s="48"/>
-      <c r="Q43" s="48"/>
-      <c r="R43" s="48"/>
-      <c r="S43" s="31"/>
-      <c r="T43" s="31"/>
-      <c r="U43" s="31"/>
+      <c r="M43" s="29"/>
+      <c r="N43" s="58"/>
+      <c r="P43" s="46"/>
+      <c r="Q43" s="46"/>
+      <c r="R43" s="46"/>
+      <c r="S43" s="29"/>
+      <c r="T43" s="29"/>
+      <c r="U43" s="29"/>
       <c r="V43" s="20"/>
-      <c r="W43" s="29"/>
+      <c r="W43" s="27"/>
     </row>
     <row r="44" spans="1:23">
-      <c r="A44" s="66" t="s">
+      <c r="A44" s="62" t="s">
         <v>190</v>
       </c>
       <c r="B44" s="11" t="s">
@@ -3329,7 +3396,7 @@
       <c r="C44" s="11" t="s">
         <v>23</v>
       </c>
-      <c r="D44" s="39" t="s">
+      <c r="D44" s="37" t="s">
         <v>90</v>
       </c>
       <c r="E44" s="11" t="s">
@@ -3365,13 +3432,13 @@
       <c r="O44" s="11" t="s">
         <v>91</v>
       </c>
-      <c r="P44" s="49" t="s">
+      <c r="P44" s="47" t="s">
         <v>239</v>
       </c>
-      <c r="Q44" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="R44" s="49" t="s">
+      <c r="Q44" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="R44" s="47" t="s">
         <v>140</v>
       </c>
       <c r="S44" s="11">
@@ -3387,7 +3454,7 @@
       <c r="W44" s="20"/>
     </row>
     <row r="45" spans="1:23">
-      <c r="A45" s="66" t="s">
+      <c r="A45" s="62" t="s">
         <v>191</v>
       </c>
       <c r="B45" s="11" t="s">
@@ -3396,7 +3463,7 @@
       <c r="C45" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D45" s="30" t="s">
+      <c r="D45" s="28" t="s">
         <v>121</v>
       </c>
       <c r="E45" s="11" t="s">
@@ -3432,13 +3499,13 @@
       <c r="O45" s="11" t="s">
         <v>29</v>
       </c>
-      <c r="P45" s="49" t="s">
+      <c r="P45" s="47" t="s">
         <v>26</v>
       </c>
-      <c r="Q45" s="49" t="s">
-        <v>136</v>
-      </c>
-      <c r="R45" s="49" t="s">
+      <c r="Q45" s="47" t="s">
+        <v>136</v>
+      </c>
+      <c r="R45" s="47" t="s">
         <v>139</v>
       </c>
       <c r="S45" s="11">
@@ -3454,7 +3521,7 @@
       <c r="W45" s="20"/>
     </row>
     <row r="46" spans="1:23">
-      <c r="A46" s="66" t="s">
+      <c r="A46" s="62" t="s">
         <v>192</v>
       </c>
       <c r="B46" s="11" t="s">
@@ -3463,7 +3530,7 @@
       <c r="C46" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D46" s="30" t="s">
+      <c r="D46" s="28" t="s">
         <v>79</v>
       </c>
       <c r="E46" s="11" t="s">
@@ -3491,9 +3558,9 @@
       <c r="M46" s="3"/>
       <c r="N46" s="3"/>
       <c r="O46" s="3"/>
-      <c r="P46" s="50"/>
-      <c r="Q46" s="50"/>
-      <c r="R46" s="50"/>
+      <c r="P46" s="48"/>
+      <c r="Q46" s="48"/>
+      <c r="R46" s="48"/>
       <c r="S46" s="21"/>
       <c r="T46" s="21"/>
       <c r="U46" s="21"/>
@@ -3501,7 +3568,7 @@
       <c r="W46" s="20"/>
     </row>
     <row r="47" spans="1:23">
-      <c r="A47" s="66" t="s">
+      <c r="A47" s="62" t="s">
         <v>193</v>
       </c>
       <c r="B47" s="19" t="s">
@@ -3510,7 +3577,7 @@
       <c r="C47" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D47" s="38" t="s">
+      <c r="D47" s="36" t="s">
         <v>265</v>
       </c>
       <c r="E47" s="19" t="s">
@@ -3546,13 +3613,13 @@
       <c r="O47" s="19" t="s">
         <v>22</v>
       </c>
-      <c r="P47" s="44" t="s">
+      <c r="P47" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q47" s="44" t="s">
+      <c r="Q47" s="42" t="s">
         <v>135</v>
       </c>
-      <c r="R47" s="44" t="s">
+      <c r="R47" s="42" t="s">
         <v>137</v>
       </c>
       <c r="S47" s="19">
@@ -3568,7 +3635,7 @@
       <c r="W47" s="20"/>
     </row>
     <row r="48" spans="1:23">
-      <c r="A48" s="66" t="s">
+      <c r="A48" s="62" t="s">
         <v>194</v>
       </c>
       <c r="B48" s="19" t="s">
@@ -3577,7 +3644,7 @@
       <c r="C48" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D48" s="38" t="s">
+      <c r="D48" s="36" t="s">
         <v>3</v>
       </c>
       <c r="E48" s="19" t="s">
@@ -3605,9 +3672,9 @@
       <c r="M48" s="3"/>
       <c r="N48" s="3"/>
       <c r="O48" s="21"/>
-      <c r="P48" s="54"/>
-      <c r="Q48" s="54"/>
-      <c r="R48" s="54"/>
+      <c r="P48" s="52"/>
+      <c r="Q48" s="52"/>
+      <c r="R48" s="52"/>
       <c r="S48" s="3"/>
       <c r="T48" s="3"/>
       <c r="U48" s="3"/>
@@ -3615,7 +3682,7 @@
       <c r="W48" s="20"/>
     </row>
     <row r="49" spans="1:23">
-      <c r="A49" s="66" t="s">
+      <c r="A49" s="62" t="s">
         <v>195</v>
       </c>
       <c r="B49" s="17" t="s">
@@ -3624,7 +3691,7 @@
       <c r="C49" s="17" t="s">
         <v>23</v>
       </c>
-      <c r="D49" s="55" t="s">
+      <c r="D49" s="53" t="s">
         <v>244</v>
       </c>
       <c r="E49" s="17" t="s">
@@ -3660,13 +3727,13 @@
       <c r="O49" s="17" t="s">
         <v>93</v>
       </c>
-      <c r="P49" s="60" t="s">
+      <c r="P49" s="56" t="s">
         <v>245</v>
       </c>
-      <c r="Q49" s="60" t="s">
+      <c r="Q49" s="56" t="s">
         <v>135</v>
       </c>
-      <c r="R49" s="60" t="s">
+      <c r="R49" s="56" t="s">
         <v>142</v>
       </c>
       <c r="S49" s="17">
@@ -3682,7 +3749,7 @@
       <c r="W49" s="20"/>
     </row>
     <row r="50" spans="1:23">
-      <c r="A50" s="66" t="s">
+      <c r="A50" s="62" t="s">
         <v>196</v>
       </c>
       <c r="B50" s="17" t="s">
@@ -3691,13 +3758,13 @@
       <c r="C50" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D50" s="40" t="s">
+      <c r="D50" s="38" t="s">
         <v>124</v>
       </c>
-      <c r="E50" s="60" t="s">
+      <c r="E50" s="70" t="s">
         <v>245</v>
       </c>
-      <c r="F50" s="60" t="s">
+      <c r="F50" s="70" t="s">
         <v>6</v>
       </c>
       <c r="G50" s="17" t="s">
@@ -3719,9 +3786,9 @@
       <c r="M50" s="3"/>
       <c r="N50" s="3"/>
       <c r="O50" s="3"/>
-      <c r="P50" s="50"/>
-      <c r="Q50" s="50"/>
-      <c r="R50" s="50"/>
+      <c r="P50" s="48"/>
+      <c r="Q50" s="48"/>
+      <c r="R50" s="48"/>
       <c r="S50" s="21"/>
       <c r="T50" s="21"/>
       <c r="U50" s="21"/>
@@ -3729,7 +3796,7 @@
       <c r="W50" s="20"/>
     </row>
     <row r="51" spans="1:23">
-      <c r="A51" s="66" t="s">
+      <c r="A51" s="62" t="s">
         <v>197</v>
       </c>
       <c r="B51" s="11" t="s">
@@ -3738,7 +3805,7 @@
       <c r="C51" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D51" s="41" t="s">
+      <c r="D51" s="39" t="s">
         <v>125</v>
       </c>
       <c r="E51" s="11" t="s">
@@ -3774,13 +3841,13 @@
       <c r="O51" s="11" t="s">
         <v>95</v>
       </c>
-      <c r="P51" s="46" t="s">
+      <c r="P51" s="44" t="s">
         <v>239</v>
       </c>
-      <c r="Q51" s="46" t="s">
-        <v>136</v>
-      </c>
-      <c r="R51" s="46" t="s">
+      <c r="Q51" s="44" t="s">
+        <v>136</v>
+      </c>
+      <c r="R51" s="44" t="s">
         <v>140</v>
       </c>
       <c r="S51" s="11">
@@ -3796,7 +3863,7 @@
       <c r="W51" s="20"/>
     </row>
     <row r="52" spans="1:23">
-      <c r="A52" s="66" t="s">
+      <c r="A52" s="62" t="s">
         <v>198</v>
       </c>
       <c r="B52" s="11" t="s">
@@ -3805,7 +3872,7 @@
       <c r="C52" s="11" t="s">
         <v>24</v>
       </c>
-      <c r="D52" s="30" t="s">
+      <c r="D52" s="28" t="s">
         <v>80</v>
       </c>
       <c r="E52" s="11" t="s">
@@ -3833,26 +3900,26 @@
       <c r="M52" s="2"/>
       <c r="N52" s="2"/>
       <c r="O52" s="2"/>
-      <c r="P52" s="51"/>
-      <c r="Q52" s="51"/>
-      <c r="R52" s="51"/>
+      <c r="P52" s="49"/>
+      <c r="Q52" s="49"/>
+      <c r="R52" s="49"/>
       <c r="S52" s="2"/>
       <c r="T52" s="2"/>
       <c r="U52" s="2"/>
-      <c r="V52" s="28"/>
+      <c r="V52" s="26"/>
       <c r="W52" s="6"/>
     </row>
     <row r="53" spans="1:23">
-      <c r="A53" s="66" t="s">
+      <c r="A53" s="62" t="s">
         <v>199</v>
       </c>
-      <c r="B53" s="44" t="s">
+      <c r="B53" s="42" t="s">
         <v>114</v>
       </c>
       <c r="C53" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D53" s="38" t="s">
+      <c r="D53" s="36" t="s">
         <v>101</v>
       </c>
       <c r="E53" s="19" t="s">
@@ -3876,7 +3943,7 @@
       <c r="K53" s="19" t="s">
         <v>253</v>
       </c>
-      <c r="L53" s="44" t="s">
+      <c r="L53" s="42" t="s">
         <v>96</v>
       </c>
       <c r="M53" s="19" t="s">
@@ -3888,13 +3955,13 @@
       <c r="O53" s="19" t="s">
         <v>100</v>
       </c>
-      <c r="P53" s="44" t="s">
+      <c r="P53" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q53" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R53" s="44" t="s">
+      <c r="Q53" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="R53" s="42" t="s">
         <v>139</v>
       </c>
       <c r="S53" s="19">
@@ -3906,20 +3973,20 @@
       <c r="U53" s="19" t="s">
         <v>260</v>
       </c>
-      <c r="V53" s="56"/>
+      <c r="V53" s="54"/>
       <c r="W53" s="6"/>
     </row>
     <row r="54" spans="1:23">
-      <c r="A54" s="66" t="s">
+      <c r="A54" s="62" t="s">
         <v>200</v>
       </c>
-      <c r="B54" s="44" t="s">
+      <c r="B54" s="42" t="s">
         <v>115</v>
       </c>
       <c r="C54" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D54" s="38" t="s">
+      <c r="D54" s="36" t="s">
         <v>2</v>
       </c>
       <c r="E54" s="19" t="s">
@@ -3943,7 +4010,7 @@
       <c r="K54" s="19" t="s">
         <v>251</v>
       </c>
-      <c r="L54" s="44" t="s">
+      <c r="L54" s="42" t="s">
         <v>97</v>
       </c>
       <c r="M54" s="19" t="s">
@@ -3955,38 +4022,38 @@
       <c r="O54" s="19" t="s">
         <v>133</v>
       </c>
-      <c r="P54" s="44" t="s">
+      <c r="P54" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q54" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R54" s="44" t="s">
+      <c r="Q54" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="R54" s="42" t="s">
         <v>140</v>
       </c>
-      <c r="S54" s="25">
+      <c r="S54" s="24">
         <v>1</v>
       </c>
-      <c r="T54" s="25" t="s">
+      <c r="T54" s="24" t="s">
         <v>134</v>
       </c>
-      <c r="U54" s="25" t="s">
+      <c r="U54" s="24" t="s">
         <v>251</v>
       </c>
-      <c r="V54" s="56"/>
+      <c r="V54" s="54"/>
       <c r="W54" s="6"/>
     </row>
     <row r="55" spans="1:23">
-      <c r="A55" s="66" t="s">
+      <c r="A55" s="62" t="s">
         <v>201</v>
       </c>
-      <c r="B55" s="44" t="s">
+      <c r="B55" s="42" t="s">
         <v>116</v>
       </c>
       <c r="C55" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D55" s="38" t="s">
+      <c r="D55" s="36" t="s">
         <v>20</v>
       </c>
       <c r="E55" s="19" t="s">
@@ -4010,7 +4077,7 @@
       <c r="K55" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="L55" s="44" t="s">
+      <c r="L55" s="42" t="s">
         <v>98</v>
       </c>
       <c r="M55" s="19" t="s">
@@ -4022,13 +4089,13 @@
       <c r="O55" s="19" t="s">
         <v>128</v>
       </c>
-      <c r="P55" s="44" t="s">
+      <c r="P55" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q55" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R55" s="44" t="s">
+      <c r="Q55" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="R55" s="42" t="s">
         <v>138</v>
       </c>
       <c r="S55" s="19">
@@ -4040,20 +4107,20 @@
       <c r="U55" s="19" t="s">
         <v>52</v>
       </c>
-      <c r="V55" s="56"/>
+      <c r="V55" s="54"/>
       <c r="W55" s="6"/>
     </row>
     <row r="56" spans="1:23">
-      <c r="A56" s="66" t="s">
+      <c r="A56" s="62" t="s">
         <v>202</v>
       </c>
-      <c r="B56" s="44" t="s">
+      <c r="B56" s="42" t="s">
         <v>88</v>
       </c>
       <c r="C56" s="19" t="s">
         <v>24</v>
       </c>
-      <c r="D56" s="38" t="s">
+      <c r="D56" s="36" t="s">
         <v>81</v>
       </c>
       <c r="E56" s="19" t="s">
@@ -4081,26 +4148,26 @@
       <c r="M56" s="22"/>
       <c r="N56" s="22"/>
       <c r="O56" s="22"/>
-      <c r="P56" s="28"/>
-      <c r="Q56" s="28"/>
-      <c r="R56" s="28"/>
+      <c r="P56" s="26"/>
+      <c r="Q56" s="26"/>
+      <c r="R56" s="26"/>
       <c r="S56" s="2"/>
       <c r="T56" s="2"/>
       <c r="U56" s="2"/>
-      <c r="V56" s="56"/>
+      <c r="V56" s="54"/>
       <c r="W56" s="6"/>
     </row>
     <row r="57" spans="1:23">
-      <c r="A57" s="66" t="s">
+      <c r="A57" s="62" t="s">
         <v>203</v>
       </c>
-      <c r="B57" s="44" t="s">
+      <c r="B57" s="42" t="s">
         <v>117</v>
       </c>
       <c r="C57" s="19" t="s">
         <v>23</v>
       </c>
-      <c r="D57" s="42" t="s">
+      <c r="D57" s="40" t="s">
         <v>102</v>
       </c>
       <c r="E57" s="19" t="s">
@@ -4136,13 +4203,13 @@
       <c r="O57" s="19" t="s">
         <v>21</v>
       </c>
-      <c r="P57" s="44" t="s">
+      <c r="P57" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q57" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R57" s="44" t="s">
+      <c r="Q57" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="R57" s="42" t="s">
         <v>138</v>
       </c>
       <c r="S57" s="19">
@@ -4154,25 +4221,41 @@
       <c r="U57" s="19" t="s">
         <v>262</v>
       </c>
-      <c r="V57" s="56"/>
+      <c r="V57" s="54"/>
       <c r="W57" s="6"/>
     </row>
     <row r="58" spans="1:23">
-      <c r="A58" s="66" t="s">
+      <c r="A58" s="64" t="s">
         <v>204</v>
       </c>
-      <c r="B58" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C58" s="3"/>
-      <c r="D58" s="3"/>
-      <c r="E58" s="3"/>
-      <c r="F58" s="3"/>
-      <c r="G58" s="3"/>
-      <c r="H58" s="3"/>
-      <c r="I58" s="21"/>
-      <c r="J58" s="21"/>
-      <c r="K58" s="21"/>
+      <c r="B58" s="40" t="s">
+        <v>270</v>
+      </c>
+      <c r="C58" s="40" t="s">
+        <v>23</v>
+      </c>
+      <c r="D58" s="40" t="s">
+        <v>269</v>
+      </c>
+      <c r="E58" s="40" t="s">
+        <v>239</v>
+      </c>
+      <c r="F58" s="40" t="s">
+        <v>4</v>
+      </c>
+      <c r="G58" s="40" t="s">
+        <v>135</v>
+      </c>
+      <c r="H58" s="40"/>
+      <c r="I58" s="40">
+        <v>2</v>
+      </c>
+      <c r="J58" s="40" t="s">
+        <v>51</v>
+      </c>
+      <c r="K58" s="40" t="s">
+        <v>51</v>
+      </c>
       <c r="L58" s="3"/>
       <c r="M58" s="3"/>
       <c r="N58" s="3"/>
@@ -4183,11 +4266,11 @@
       <c r="S58" s="2"/>
       <c r="T58" s="2"/>
       <c r="U58" s="2"/>
-      <c r="V58" s="56"/>
+      <c r="V58" s="54"/>
       <c r="W58" s="6"/>
     </row>
     <row r="59" spans="1:23">
-      <c r="A59" s="66" t="s">
+      <c r="A59" s="62" t="s">
         <v>205</v>
       </c>
       <c r="B59" s="19" t="s">
@@ -4232,13 +4315,13 @@
       <c r="O59" s="19" t="s">
         <v>104</v>
       </c>
-      <c r="P59" s="44" t="s">
+      <c r="P59" s="42" t="s">
         <v>239</v>
       </c>
-      <c r="Q59" s="44" t="s">
-        <v>136</v>
-      </c>
-      <c r="R59" s="44" t="s">
+      <c r="Q59" s="42" t="s">
+        <v>136</v>
+      </c>
+      <c r="R59" s="42" t="s">
         <v>138</v>
       </c>
       <c r="S59" s="19">
@@ -4250,11 +4333,11 @@
       <c r="U59" s="19" t="s">
         <v>60</v>
       </c>
-      <c r="V59" s="56"/>
+      <c r="V59" s="54"/>
       <c r="W59" s="6"/>
     </row>
     <row r="60" spans="1:23">
-      <c r="A60" s="66" t="s">
+      <c r="A60" s="62" t="s">
         <v>206</v>
       </c>
       <c r="B60" s="17" t="s">
@@ -4263,7 +4346,7 @@
       <c r="C60" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D60" s="24" t="s">
+      <c r="D60" s="50" t="s">
         <v>106</v>
       </c>
       <c r="E60" s="17" t="s">
@@ -4272,16 +4355,20 @@
       <c r="F60" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G60" s="17"/>
-      <c r="H60" s="17"/>
-      <c r="I60" s="17" t="s">
-        <v>27</v>
+      <c r="G60" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="H60" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="I60" s="17">
+        <v>2</v>
       </c>
       <c r="J60" s="17" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="K60" s="17" t="s">
-        <v>27</v>
+        <v>51</v>
       </c>
       <c r="L60" s="17" t="s">
         <v>108</v>
@@ -4292,28 +4379,32 @@
       <c r="N60" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="O60" s="24" t="s">
+      <c r="O60" s="50" t="s">
         <v>92</v>
       </c>
       <c r="P60" s="17" t="s">
         <v>240</v>
       </c>
-      <c r="Q60" s="17"/>
-      <c r="R60" s="17"/>
-      <c r="S60" s="57" t="s">
-        <v>27</v>
-      </c>
-      <c r="T60" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="U60" s="58" t="s">
-        <v>27</v>
-      </c>
-      <c r="V60" s="56"/>
-      <c r="W60" s="59"/>
+      <c r="Q60" s="17" t="s">
+        <v>136</v>
+      </c>
+      <c r="R60" s="17" t="s">
+        <v>138</v>
+      </c>
+      <c r="S60" s="17">
+        <v>2</v>
+      </c>
+      <c r="T60" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="U60" s="17" t="s">
+        <v>51</v>
+      </c>
+      <c r="V60" s="54"/>
+      <c r="W60" s="55"/>
     </row>
     <row r="61" spans="1:23">
-      <c r="A61" s="66" t="s">
+      <c r="A61" s="62" t="s">
         <v>207</v>
       </c>
       <c r="B61" s="19" t="s">
@@ -4340,10 +4431,10 @@
       <c r="I61" s="19">
         <v>4</v>
       </c>
-      <c r="J61" s="21" t="s">
+      <c r="J61" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="K61" s="21" t="s">
+      <c r="K61" s="24" t="s">
         <v>27</v>
       </c>
       <c r="L61" s="12" t="s">
@@ -4376,54 +4467,88 @@
       <c r="U61" s="13" t="s">
         <v>27</v>
       </c>
-      <c r="V61" s="56"/>
-      <c r="W61" s="59"/>
+      <c r="V61" s="54"/>
+      <c r="W61" s="55"/>
     </row>
     <row r="62" spans="1:23">
-      <c r="A62" s="66" t="s">
+      <c r="A62" s="64" t="s">
         <v>208</v>
       </c>
-      <c r="B62" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C62" s="3"/>
-      <c r="D62" s="3"/>
-      <c r="E62" s="3"/>
-      <c r="F62" s="3"/>
-      <c r="G62" s="3"/>
-      <c r="H62" s="3"/>
-      <c r="I62" s="21"/>
-      <c r="J62" s="21"/>
-      <c r="K62" s="21"/>
-      <c r="L62" s="3"/>
+      <c r="B62" s="17" t="s">
+        <v>288</v>
+      </c>
+      <c r="C62" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D62" s="17" t="s">
+        <v>289</v>
+      </c>
+      <c r="E62" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="F62" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G62" s="17"/>
+      <c r="H62" s="17"/>
+      <c r="I62" s="17"/>
+      <c r="J62" s="17"/>
+      <c r="K62" s="17"/>
+      <c r="L62" s="3" t="s">
+        <v>290</v>
+      </c>
       <c r="M62" s="3"/>
-      <c r="N62" s="3"/>
-      <c r="O62" s="3"/>
-      <c r="P62" s="2"/>
+      <c r="N62" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O62" s="3" t="s">
+        <v>291</v>
+      </c>
+      <c r="P62" s="2" t="s">
+        <v>240</v>
+      </c>
       <c r="Q62" s="2"/>
       <c r="R62" s="2"/>
       <c r="S62" s="2"/>
       <c r="T62" s="2"/>
       <c r="U62" s="2"/>
-      <c r="V62" s="56"/>
+      <c r="V62" s="54"/>
       <c r="W62" s="6"/>
     </row>
     <row r="63" spans="1:23">
-      <c r="A63" s="66" t="s">
+      <c r="A63" s="62" t="s">
         <v>209</v>
       </c>
-      <c r="B63" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C63" s="3"/>
-      <c r="D63" s="3"/>
-      <c r="E63" s="3"/>
-      <c r="F63" s="3"/>
-      <c r="G63" s="3"/>
-      <c r="H63" s="3"/>
-      <c r="I63" s="21"/>
-      <c r="J63" s="21"/>
-      <c r="K63" s="21"/>
+      <c r="B63" s="50" t="s">
+        <v>271</v>
+      </c>
+      <c r="C63" s="50" t="s">
+        <v>24</v>
+      </c>
+      <c r="D63" s="50" t="s">
+        <v>272</v>
+      </c>
+      <c r="E63" s="50" t="s">
+        <v>245</v>
+      </c>
+      <c r="F63" s="50" t="s">
+        <v>6</v>
+      </c>
+      <c r="G63" s="50" t="s">
+        <v>136</v>
+      </c>
+      <c r="H63" s="50" t="s">
+        <v>140</v>
+      </c>
+      <c r="I63" s="50">
+        <v>1</v>
+      </c>
+      <c r="J63" s="50" t="s">
+        <v>70</v>
+      </c>
+      <c r="K63" s="50" t="s">
+        <v>60</v>
+      </c>
       <c r="L63" s="3"/>
       <c r="M63" s="3"/>
       <c r="N63" s="3"/>
@@ -4434,11 +4559,11 @@
       <c r="S63" s="2"/>
       <c r="T63" s="2"/>
       <c r="U63" s="2"/>
-      <c r="V63" s="56"/>
+      <c r="V63" s="54"/>
       <c r="W63" s="6"/>
     </row>
     <row r="64" spans="1:23">
-      <c r="A64" s="66" t="s">
+      <c r="A64" s="62" t="s">
         <v>210</v>
       </c>
       <c r="B64" s="17" t="s">
@@ -4447,8 +4572,8 @@
       <c r="C64" s="17" t="s">
         <v>24</v>
       </c>
-      <c r="D64" s="52" t="s">
-        <v>267</v>
+      <c r="D64" s="50" t="s">
+        <v>266</v>
       </c>
       <c r="E64" s="17" t="s">
         <v>240</v>
@@ -4456,7 +4581,9 @@
       <c r="F64" s="17" t="s">
         <v>6</v>
       </c>
-      <c r="G64" s="17"/>
+      <c r="G64" s="17" t="s">
+        <v>136</v>
+      </c>
       <c r="H64" s="17" t="s">
         <v>138</v>
       </c>
@@ -4479,68 +4606,137 @@
       <c r="S64" s="2"/>
       <c r="T64" s="2"/>
       <c r="U64" s="2"/>
-      <c r="V64" s="56"/>
+      <c r="V64" s="54"/>
       <c r="W64" s="6"/>
     </row>
     <row r="65" spans="1:23">
-      <c r="A65" s="66" t="s">
+      <c r="A65" s="62" t="s">
         <v>211</v>
       </c>
-      <c r="B65" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C65" s="3"/>
-      <c r="D65" s="3"/>
-      <c r="E65" s="3"/>
-      <c r="F65" s="3"/>
-      <c r="G65" s="3"/>
-      <c r="H65" s="3"/>
-      <c r="I65" s="21"/>
-      <c r="J65" s="21"/>
-      <c r="L65" s="3"/>
-      <c r="M65" s="3"/>
-      <c r="N65" s="3"/>
-      <c r="O65" s="3"/>
-      <c r="P65" s="2"/>
-      <c r="Q65" s="2"/>
-      <c r="R65" s="2"/>
-      <c r="S65" s="2"/>
-      <c r="T65" s="2"/>
-      <c r="U65" s="2"/>
-      <c r="V65" s="56"/>
+      <c r="B65" s="17" t="s">
+        <v>276</v>
+      </c>
+      <c r="C65" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D65" s="17" t="s">
+        <v>273</v>
+      </c>
+      <c r="E65" s="17" t="s">
+        <v>245</v>
+      </c>
+      <c r="F65" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G65" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="H65" s="17">
+        <v>5</v>
+      </c>
+      <c r="I65" s="17">
+        <v>2</v>
+      </c>
+      <c r="J65" s="17"/>
+      <c r="K65" s="17"/>
+      <c r="L65" s="17" t="s">
+        <v>274</v>
+      </c>
+      <c r="M65" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="N65" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="O65" s="17" t="s">
+        <v>275</v>
+      </c>
+      <c r="P65" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q65" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="R65" s="17">
+        <v>5</v>
+      </c>
+      <c r="S65" s="17">
+        <v>2</v>
+      </c>
+      <c r="T65" s="17"/>
+      <c r="U65" s="17"/>
+      <c r="V65" s="54"/>
       <c r="W65" s="6"/>
     </row>
     <row r="66" spans="1:23">
-      <c r="A66" s="66" t="s">
+      <c r="A66" s="62" t="s">
         <v>212</v>
       </c>
-      <c r="B66" s="3" t="s">
-        <v>89</v>
-      </c>
-      <c r="C66" s="3"/>
-      <c r="D66" s="3"/>
-      <c r="E66" s="3"/>
-      <c r="F66" s="3"/>
-      <c r="G66" s="3"/>
-      <c r="H66" s="3"/>
-      <c r="I66" s="21"/>
-      <c r="J66" s="21"/>
-      <c r="K66" s="21"/>
-      <c r="L66" s="3"/>
-      <c r="M66" s="3"/>
-      <c r="N66" s="3"/>
-      <c r="O66" s="3"/>
-      <c r="P66" s="2"/>
-      <c r="Q66" s="2"/>
-      <c r="R66" s="2"/>
-      <c r="S66" s="2"/>
-      <c r="T66" s="2"/>
-      <c r="U66" s="2"/>
-      <c r="V66" s="56"/>
+      <c r="B66" s="17" t="s">
+        <v>277</v>
+      </c>
+      <c r="C66" s="17" t="s">
+        <v>24</v>
+      </c>
+      <c r="D66" s="17" t="s">
+        <v>278</v>
+      </c>
+      <c r="E66" s="17" t="s">
+        <v>239</v>
+      </c>
+      <c r="F66" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G66" s="17" t="s">
+        <v>135</v>
+      </c>
+      <c r="H66" s="17">
+        <v>7</v>
+      </c>
+      <c r="I66" s="17">
+        <v>2</v>
+      </c>
+      <c r="J66" s="17" t="s">
+        <v>57</v>
+      </c>
+      <c r="K66" s="17" t="s">
+        <v>279</v>
+      </c>
+      <c r="L66" s="19" t="s">
+        <v>280</v>
+      </c>
+      <c r="M66" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="N66" s="19" t="s">
+        <v>4</v>
+      </c>
+      <c r="O66" s="19" t="s">
+        <v>281</v>
+      </c>
+      <c r="P66" s="19" t="s">
+        <v>239</v>
+      </c>
+      <c r="Q66" s="19" t="s">
+        <v>135</v>
+      </c>
+      <c r="R66" s="19">
+        <v>7</v>
+      </c>
+      <c r="S66" s="19">
+        <v>2</v>
+      </c>
+      <c r="T66" s="19" t="s">
+        <v>57</v>
+      </c>
+      <c r="U66" s="19" t="s">
+        <v>279</v>
+      </c>
+      <c r="V66" s="54"/>
       <c r="W66" s="6"/>
     </row>
     <row r="67" spans="1:23">
-      <c r="A67" s="66" t="s">
+      <c r="A67" s="62" t="s">
         <v>213</v>
       </c>
       <c r="B67" s="19" t="s">
@@ -4603,84 +4799,94 @@
       <c r="U67" s="19" t="s">
         <v>62</v>
       </c>
-      <c r="V67" s="56"/>
+      <c r="V67" s="54"/>
       <c r="W67" s="6"/>
     </row>
     <row r="68" spans="1:23">
-      <c r="A68" s="66" t="s">
+      <c r="A68" s="64" t="s">
         <v>214</v>
       </c>
       <c r="B68" s="19" t="s">
         <v>112</v>
       </c>
       <c r="C68" s="19" t="s">
+        <v>23</v>
+      </c>
+      <c r="D68" s="19" t="s">
+        <v>292</v>
+      </c>
+      <c r="E68" s="65"/>
+      <c r="F68" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="G68" s="65"/>
+      <c r="H68" s="19"/>
+      <c r="I68" s="19"/>
+      <c r="J68" s="19"/>
+      <c r="K68" s="19"/>
+      <c r="L68" s="3" t="s">
+        <v>282</v>
+      </c>
+      <c r="M68" s="3" t="s">
         <v>24</v>
       </c>
-      <c r="D68" s="19" t="s">
-        <v>266</v>
-      </c>
-      <c r="E68" s="25" t="s">
-        <v>245</v>
-      </c>
-      <c r="F68" s="25" t="s">
-        <v>4</v>
-      </c>
-      <c r="G68" s="25" t="s">
-        <v>136</v>
-      </c>
-      <c r="H68" s="19" t="s">
-        <v>138</v>
-      </c>
-      <c r="I68" s="19">
-        <v>4</v>
-      </c>
-      <c r="J68" s="19" t="s">
-        <v>248</v>
-      </c>
-      <c r="K68" s="19" t="s">
-        <v>54</v>
-      </c>
-      <c r="L68" s="3"/>
-      <c r="M68" s="3"/>
       <c r="N68" s="3"/>
       <c r="O68" s="3"/>
       <c r="P68" s="2"/>
-      <c r="Q68" s="2"/>
-      <c r="R68" s="2"/>
-      <c r="S68" s="2"/>
-      <c r="T68" s="2"/>
-      <c r="U68" s="2"/>
-      <c r="V68" s="45"/>
-      <c r="W68" s="26"/>
+      <c r="Q68" s="24" t="s">
+        <v>136</v>
+      </c>
+      <c r="R68" s="19" t="s">
+        <v>138</v>
+      </c>
+      <c r="S68" s="19">
+        <v>4</v>
+      </c>
+      <c r="T68" s="19" t="s">
+        <v>248</v>
+      </c>
+      <c r="U68" s="19" t="s">
+        <v>54</v>
+      </c>
+      <c r="V68" s="43"/>
+      <c r="W68" s="25"/>
     </row>
     <row r="69" spans="1:23">
-      <c r="A69" s="67" t="s">
+      <c r="A69" s="66" t="s">
         <v>235</v>
       </c>
-      <c r="B69" s="22" t="s">
+      <c r="B69" s="17" t="s">
         <v>89</v>
       </c>
-      <c r="C69" s="22"/>
-      <c r="D69" s="22"/>
-      <c r="E69" s="22"/>
-      <c r="F69" s="22"/>
-      <c r="G69" s="22"/>
-      <c r="H69" s="22"/>
-      <c r="I69" s="27"/>
-      <c r="J69" s="27"/>
-      <c r="K69" s="27"/>
+      <c r="C69" s="17" t="s">
+        <v>23</v>
+      </c>
+      <c r="D69" s="17" t="s">
+        <v>287</v>
+      </c>
+      <c r="E69" s="17" t="s">
+        <v>240</v>
+      </c>
+      <c r="F69" s="17" t="s">
+        <v>6</v>
+      </c>
+      <c r="G69" s="17"/>
+      <c r="H69" s="17"/>
+      <c r="I69" s="17"/>
+      <c r="J69" s="17"/>
+      <c r="K69" s="17"/>
       <c r="L69" s="22"/>
       <c r="M69" s="22"/>
       <c r="N69" s="22"/>
       <c r="O69" s="22"/>
-      <c r="P69" s="28"/>
-      <c r="Q69" s="28"/>
-      <c r="R69" s="28"/>
-      <c r="S69" s="28"/>
-      <c r="T69" s="28"/>
-      <c r="U69" s="28"/>
-      <c r="V69" s="28"/>
-      <c r="W69" s="28"/>
+      <c r="P69" s="26"/>
+      <c r="Q69" s="26"/>
+      <c r="R69" s="26"/>
+      <c r="S69" s="26"/>
+      <c r="T69" s="26"/>
+      <c r="U69" s="26"/>
+      <c r="V69" s="26"/>
+      <c r="W69" s="26"/>
     </row>
     <row r="70" spans="1:23">
       <c r="A70" s="68" t="s">
@@ -4689,13 +4895,48 @@
       <c r="B70" s="22" t="s">
         <v>89</v>
       </c>
+      <c r="C70" s="69" t="s">
+        <v>24</v>
+      </c>
     </row>
     <row r="71" spans="1:23">
       <c r="A71" s="68" t="s">
         <v>237</v>
       </c>
-      <c r="B71" s="22" t="s">
-        <v>89</v>
+      <c r="B71" s="65" t="s">
+        <v>285</v>
+      </c>
+      <c r="C71" s="65" t="s">
+        <v>23</v>
+      </c>
+      <c r="D71" s="65" t="s">
+        <v>286</v>
+      </c>
+      <c r="E71" s="65"/>
+      <c r="F71" s="65" t="s">
+        <v>4</v>
+      </c>
+      <c r="G71" s="65"/>
+      <c r="H71" s="65"/>
+      <c r="I71" s="65"/>
+      <c r="J71" s="65"/>
+      <c r="K71" s="65"/>
+    </row>
+    <row r="72" spans="1:23">
+      <c r="A72" s="68" t="s">
+        <v>268</v>
+      </c>
+      <c r="B72" s="22" t="s">
+        <v>283</v>
+      </c>
+      <c r="C72" s="67" t="s">
+        <v>24</v>
+      </c>
+      <c r="L72" t="s">
+        <v>284</v>
+      </c>
+      <c r="M72" t="s">
+        <v>23</v>
       </c>
     </row>
   </sheetData>
@@ -4708,6 +4949,6 @@
   </customSheetViews>
   <phoneticPr fontId="8" type="noConversion"/>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
-  <pageSetup paperSize="8" scale="49" orientation="landscape" horizontalDpi="0" verticalDpi="0"/>
+  <pageSetup paperSize="8" scale="49" orientation="landscape" r:id="rId1"/>
 </worksheet>
 </file>
</xml_diff>